<commit_message>
changes to the template
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="122">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -108,12 +108,18 @@
     <t xml:space="preserve">L&amp;T Spaza Affordable</t>
   </si>
   <si>
+    <t xml:space="preserve">Price, Survey, Availability, SOS, Count</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">SSD IC</t>
   </si>
   <si>
+    <t xml:space="preserve">Price, Survey, Availability</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
@@ -135,15 +141,27 @@
     <t xml:space="preserve">Pricing Compliance</t>
   </si>
   <si>
+    <t xml:space="preserve">Price</t>
+  </si>
+  <si>
     <t xml:space="preserve">Activation</t>
   </si>
   <si>
+    <t xml:space="preserve">Survey</t>
+  </si>
+  <si>
     <t xml:space="preserve">Availability and Pricing of ALL Key Packs </t>
   </si>
   <si>
+    <t xml:space="preserve">??</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOC: Sparletta, Twist and Stills</t>
   </si>
   <si>
+    <t xml:space="preserve">Planogram</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atomic KPI Name</t>
   </si>
   <si>
@@ -283,9 +301,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pricing Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Survey</t>
   </si>
   <si>
     <t xml:space="preserve">type avia</t>
@@ -407,7 +422,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -429,12 +444,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -492,7 +501,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,17 +525,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,14 +592,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -672,7 +676,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,23 +784,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.353488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.9209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -803,16 +809,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -822,21 +831,27 @@
       <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="n">
         <v>11</v>
       </c>
     </row>
@@ -845,13 +860,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="n">
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="n">
         <v>8</v>
       </c>
     </row>
@@ -860,13 +878,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="n">
         <v>6</v>
       </c>
     </row>
@@ -875,13 +896,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="n">
         <v>8</v>
       </c>
     </row>
@@ -890,13 +914,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="n">
         <v>8</v>
       </c>
     </row>
@@ -905,13 +932,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="n">
         <v>4</v>
       </c>
     </row>
@@ -920,56 +950,68 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="F11" s="7" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="n">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -997,9 +1039,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,18 +1049,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>100</v>
@@ -1049,19 +1091,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.353488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.8093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.66046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.7767441860465"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.78604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,118 +1111,118 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>200</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>5</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1190,201 +1232,201 @@
         <v>5</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>7</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>9</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>13</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>10.5</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>12.99</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>14</v>
@@ -1393,21 +1435,21 @@
         <v>3</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>17</v>
@@ -1416,13 +1458,13 @@
         <v>3</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1450,14 +1492,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,25 +1507,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1491,304 +1533,304 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1816,23 +1858,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.4"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.0279069767442"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.306976744186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,52 +1882,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,19 +1935,19 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>1</v>
@@ -1914,13 +1956,13 @@
         <v>2</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,10 +1970,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
@@ -1943,142 +1985,142 @@
         <v>5</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2106,19 +2148,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.1348837209302"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7488372093023"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,40 +2168,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,25 +2209,25 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>50</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>30</v>
@@ -2194,10 +2236,10 @@
         <v>5</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2225,12 +2267,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,22 +2280,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,7 +2303,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>4</v>
@@ -2270,13 +2312,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,7 +2326,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>3</v>
@@ -2293,13 +2335,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,7 +2349,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -2316,13 +2358,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drafting sos, amending tests
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="132">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -244,6 +244,9 @@
     <t xml:space="preserve">type avia</t>
   </si>
   <si>
+    <t xml:space="preserve">Template Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brand strips in coolers (CCBSA &amp; Dealer Owned Coolers)</t>
   </si>
   <si>
@@ -397,10 +400,10 @@
     <t xml:space="preserve">Water, KO PRODUCTS</t>
   </si>
   <si>
+    <t xml:space="preserve">Category, Manufacturer_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Template Name</t>
   </si>
   <si>
     <t xml:space="preserve">Min 4 x Cooler Doors</t>
@@ -667,13 +670,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.6232558139535"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.9767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,9 +915,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.4837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,19 +967,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="85.7720930232558"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="63.6232558139535"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="88.3581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="65.4697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,28 +1375,28 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="97.2186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="100.172093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.38604651162791"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="77.1581395348837"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="79.3767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,7 +1410,7 @@
         <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>35</v>
@@ -1451,20 +1454,20 @@
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -1481,7 +1484,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
       <c r="P2" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,10 +1492,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>47</v>
@@ -1510,7 +1513,7 @@
         <v>51</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,13 +1521,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>61</v>
@@ -1544,10 +1547,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>2</v>
@@ -1564,10 +1567,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>2</v>
@@ -1584,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>2</v>
@@ -1604,10 +1607,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>2</v>
@@ -1624,10 +1627,10 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>2</v>
@@ -1639,7 +1642,7 @@
         <v>51</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1661,20 +1664,21 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="71.9906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.8186046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.2046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,10 +1689,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>41</v>
@@ -1708,10 +1712,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>10</v>
@@ -1728,10 +1732,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>50</v>
@@ -1745,10 +1749,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>50</v>
@@ -1762,10 +1766,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>50</v>
@@ -1779,10 +1783,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>50</v>
@@ -1796,10 +1800,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>50</v>
@@ -1813,10 +1817,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>3</v>
@@ -1833,10 +1837,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3</v>
@@ -1853,10 +1857,10 @@
         <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
@@ -1873,10 +1877,10 @@
         <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>3</v>
@@ -2027,27 +2031,27 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.2976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="26.2139534883721"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.38604651162791"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.2651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2061,37 +2065,37 @@
         <v>34</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>42</v>
@@ -2108,37 +2112,37 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>30</v>
@@ -2158,37 +2162,37 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>30</v>
@@ -2200,7 +2204,7 @@
         <v>50</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,37 +2212,37 @@
         <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>35</v>
@@ -2273,14 +2277,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2288,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>31</v>
@@ -2297,7 +2301,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>42</v>
@@ -2317,7 +2321,7 @@
         <v>47</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>4</v>
@@ -2329,7 +2333,7 @@
         <v>50</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2344,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -2352,7 +2356,7 @@
         <v>50</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,7 +2367,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -2375,7 +2379,7 @@
         <v>50</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing the code along with testing
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="194">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -43,22 +43,22 @@
     <t xml:space="preserve">Dependancy</t>
   </si>
   <si>
-    <t xml:space="preserve">L&amp;T Spaza Affordable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L&amp;T Gen D Affordable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L&amp;T Spaza Mainstream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L&amp;T Gen D Mainstream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L&amp;T Spaza Premium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L&amp;T Gen D Premium</t>
+    <t xml:space="preserve">L&amp;T SPAZA AFFORDABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;T GENERAL DEALER AFFORDABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;T SPAZA MAINSTREAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;T GENERAL DEALER MAINSTREAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;T SPAZA PREMIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;T GENERAL DEALER PREMIUM</t>
   </si>
   <si>
     <t xml:space="preserve">COOLERS &amp; MERCHANDISING</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Atomic KPI Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Template Display Name </t>
+    <t xml:space="preserve">Template Display Name</t>
   </si>
   <si>
     <t xml:space="preserve">Target</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">5449000011114,5449000018601,5449000159151,5449000247285,5449000246264</t>
   </si>
   <si>
-    <t xml:space="preserve">Spaza Affordable</t>
+    <t xml:space="preserve">SPAZA AFFORDABLE</t>
   </si>
   <si>
     <t xml:space="preserve">At least one unique price in all of the scene types should reach the needed target or below</t>
@@ -247,10 +247,10 @@
     <t xml:space="preserve">5449000140906,5449000106476,5449000234605,5449000195715</t>
   </si>
   <si>
-    <t xml:space="preserve">Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver</t>
+    <t xml:space="preserve">GOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILVER</t>
   </si>
   <si>
     <t xml:space="preserve">5449000230188</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">5449000037978,5449000061768,5449000202048,5449000172167,5449000202147</t>
   </si>
   <si>
-    <t xml:space="preserve">Gen D Affordable</t>
+    <t xml:space="preserve">GENERAL DEALER AFFORDABLE</t>
   </si>
   <si>
     <t xml:space="preserve">Expected Result</t>
@@ -319,16 +319,16 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Spaza Mainstream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gen D Mainstream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaza Premium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gen D Premium</t>
+    <t xml:space="preserve">SPAZA MAINSTREAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL DEALER MAINSTREAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAZA PREMIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL DEALER PREMIUM</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler Decals per door</t>
@@ -343,196 +343,271 @@
     <t xml:space="preserve">Signage available and in good condition</t>
   </si>
   <si>
+    <t xml:space="preserve">New Product Development(NPD)/Promotional Poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x IC (300ml PET) Combo  &amp;  1 x FC (1.25L) Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparletta 2L Bulk Display with Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD 1.25L Bulk Display with Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 1 - Numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 1 - Numerator Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 1 - Denominator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 1 - Denominator Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 1 - Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 2 - Numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 2 - Numerator Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 2 - Denominator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 2 - Denominator Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition 2 - Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diets &gt; 65% out of all CCBSA SSD (CCBSA Cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCBSA Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alt_code_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FA, ST, TW, SCHW &gt;25% out of all KO Products (CCBSA Cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FANTA ORANGE, STONEY, TWIST, SCHWEPPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL SSD IC, SSD FC, Twist and Stills must be greater than 50% of All Competitor SSD IC &amp; SSD FC Flavours and Stills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCBSA &amp; DOC Coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min 4 x Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min 3 x Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min 1 x Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRONZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type avia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand strips in coolers (CCBSA &amp; Dealer Owned Coolers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one brand strip for every unique SKU under the specific brand </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min 2 facings per SKU in coolers (CCBSA &amp; Dealer Owned)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability SKU facing And</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All recognized KO Products should have at least 2 facings in every cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Availabililty of 200ml CAN, 300 ml PET, 440ml Can (CC, SP,FA, ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000011114,5449000018601,5449000159151,5449000247285,5449000246264,87126037,54492691,40822921,40822327,5449000140906,5449000106476,5449000234605,5449000195715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All recognized KO Products should have at least 2 facings in ALL of the scene types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Availabililty of: 200ml CAN, 300 ml PET (CC, SP,FA or ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000011114,5449000018601,5449000159151,5449000247285,5449000246264,87126037,54492691,40822921,40822327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Diets Availability of 200ml CAN, 300 ml PET,  440 ml Can (CZ,STZ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">90375149,5449000052131,5449000224453,5449000246295,5449000157751,5449000230188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90375149,5449000052131,5449000224453,5449000246295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD FC Availabililty of 1.25L,1.5L (CC, SP,FA, ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000009746,5449000025234,5449000027559,6001134705506,5449000000439,5449000234629,5449000052926,5449000180919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Diets Availability of: 1.5L in (CZ,STZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills - Energy Burn 500ml Availability </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Energy Pricing Poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability POSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Pricing Poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn A2 R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSM recognition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (BA) Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90492853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every unique SKU should have at least 2 facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (BAF) Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000117830,5449000117823,5449000117809,5449000117816,5449000117793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (PP) Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5060466513204,5060466513112,5060466513174,5060466513051,5060466513082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (JJ,) Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000211910,5449000211972,5449000212818,5449000212870,5449000211880,5449000211859,5449000212849,5449000212788,5449000212009,5449000211941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pricing Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pricing Board - Why Pay More</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC &amp; FC  Pricing Posters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC OBM 300ML PET,IC OBM 330ML CAN,IC OBM 440ML CAN,IC OBM 440ML PET,FC OBM 1.5L PET,FC OBM 1.25L RGB,FC OBM 1L PET,FC OBM 2.25L PET,FC OBM 2L PET</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sparletta Call Out - Pricing Poster</t>
   </si>
   <si>
-    <t xml:space="preserve">New Product Development(NPD)/Promotional Poster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x IC (300ml PET) Combo  &amp;  1 x FC (1.25L) Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 1 - Numerator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 1 - Numerator Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 1 - Denominator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 1 - Denominator Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 1 - Target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 2 - Numerator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 2 - Numerator Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 2 - Denominator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 2 - Denominator Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition 2 - Target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diets &gt; 65% out of all CCBSA SSD (CCBSA Cooler)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCBSA Cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000095046,5449000052407,5449000056276,5449000664716,5000112635362,5449000016560,5449000052131,5449000040039,5449000050205,5449000050090,5449000664709,5449000037978,5449000133328,5449000131805,5449000131812,5449000157751,5449000157768,5449000664693,5000112635560,5000112561838,5449000061768,5449000202048,5449000120960,5449000120977,5449000664761,5000112635430,5449000236371,54008014,5449000236388,5449000106704,5449000116093,5449000664785,5000112635409,5449000172167,5449000230188,5449000664792,5449000019691,5449000002969,5449000006844,5449000202147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FA, ST, TW, SCHW &gt;25% out of all KO Products (CCBSA Cooler)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000234612,5449000027559,5449000234636,54492691,5449000234599,5449000234674,5449000234582,5449000234605,5449000234643,5449000106704,5449000116093,5449000664785,5000112635409,5449000172167,5449000122544,6001134297308,5449000106261,5449000106278,5449000664884,5449000166241,6001134005507,6001134087305,5449000106322,5449000106339,5449000664846,5449000165848,5449000117977,5449000112767,6001134687307,5449000106292,5449000106308,5449000664853,5449000112774,5449000010070,5449000069429,5449000140562,5449000664723,5449000006271,5449000025234,5449000010049,40822921,5449000011527,5449000056689,5449000664754,90377235,5449000106476,5449000110305,5449000003768,90338663,5449000003201,5449000017086,5449000664747,5000112635416,5449000202048,5449000120960,5449000120977,5449000664761,5000112635430,5449000096104,5449000096807,5449000140760,5449000140777,5449000064998,5449000045515,5449000046598,5449000046604,5449000064165,5449000046581,5449000046567,6001133000138,5449000014917,5449000096098,5449000096913,5449000044808,5449000096111,5449000096784,5449000236371,54008014,5449000236388,5449000251701,5449000171351,5449000251749,5449000246479,5449000064950,6001134705506,6001134707302,5449000106421,40822327,5449000195715,5449000664808,5449000230188,5449000664792,5449000119506,5449000180889,5449000098580,5449000140791,5449000664839,6001134395509,5449000060075,5449000060082,5449000046413,5449000664822</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALL SSD IC, SSD FC, Twist and Stills must be greater than 50% of All Competitor SSD IC &amp; SSD FC Flavours and Stills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCBSA &amp; DOC Coolers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaza Affordable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min 4 x Cooler Doors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min 3 x Cooler Doors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min 1 x Cooler Doors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type avia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand strips in coolers (CCBSA &amp; Dealer Owned Coolers)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability POS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brand (new label)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At least one brand strip for every unique SKU under the specific brand </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min 2 facings per SKU in coolers (CCBSA &amp; Dealer Owned)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability SKU facing And</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All recognized KO Products should have at least 2 facings in every cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD IC Availabililty of 200ml CAN, 300 ml PET, 440ml Can (CC, SP,FA, ST)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000011114,5449000018601,5449000159151,5449000247285,5449000246264,87126037,54492691,40822921,40822327,5449000140906,5449000106476,5449000234605,5449000195715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All recognized KO Products should have at least 2 facings in ALL of the scene types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD IC Diets Availability of 200ml CAN, 300 ml PET,  440 ml Can (CZ,STZ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">90375149,5449000052131,5449000224453,5449000246295,5449000157751,5449000230188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD FC Availabililty of 1.25L,1.5L (CC, SP,FA, ST)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000009746,5449000025234,5449000027559,6001134705506,5449000000439,5449000234629,5449000052926,5449000180919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD IC Diets Availability of: 1.5L in (CZ,STZ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills - Energy Burn 500ml Availability </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Energy Pricing Poster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability POSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Pricing Poster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn A2 R10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSM recognition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (BA) Cold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90492853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Every unique SKU should have at least 2 facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (BAF) Cold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000117830,5449000117823,5449000117809,5449000117816,5449000117793</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (PP) Cold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5060466513204,5060466513112,5060466513174,5060466513051,5060466513082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills Brands/Packs: 330ml/ 440ml/500ml (JJ,) Cold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5449000211910,5449000211972,5449000212818,5449000212870,5449000211880,5449000211859,5449000212849,5449000212788,5449000212009,5449000211941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pricing Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pricing Board - Why Pay More</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC &amp; FC  Pricing Posters</t>
+    <t xml:space="preserve">Sparletta Call Out Pricing Poster 1,Sparletta Call Out Pricing Poster 2,Sparletta Call Out Pricing Poster 3,Sparletta Call Out Pricing Poster 4,Sparletta Call Out Pricing Poster 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Availabililty of: 300 ml PET,440ml Can (CC, SP,FA, ST), 440ml PET (CC, SP, FA or ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87126037,54492691,40822921,40822327,5449000140906,5449000106476,5449000234605,5449000195715,5449000664686,5449000664754,5449000234643,5449000664808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC pack sizes: 300 ml PET,440ml can (CC, SP,FA or ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87126037,54492691,40822921,40822327,5449000140906,5449000106476,5449000234605,5449000195715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Diets Brands/Packs: 300ml PET  (CZ), 440 ml Can, 440ml PET (CZ,STZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90375149,5449000157751,5449000230188,5449000664716,5449000664709,5449000664693,5449000664761,5449000664785,5449000664792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Diets Brands/Packs: 300ml PET  (CZ), 440 ml Can (CZ,STZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90375149,5449000157751,5449000230188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD FC pack sizes:1.25L(CC),1.5L,2L  (CC, SP,FA, ST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000009746,5449000025234,5449000027559,6001134705506,5449000000439,5449000234629,5449000052926,5449000180919,5449000009067,5449000010049,5449000234636,6001134707302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD FC pack sizes: 1.25L (CC),1.5L  (CC, SP, ST or FA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Diets Brands/Packs: 1.5L in (CZ/STZ),  2L (CZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000180896,5449000133335,5449000037978,5449000061768,5449000202048,5449000172167,5449000202147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Diets Brands/Packs: 1.5L in (CZ/SZ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills Availability of Burn in 500ml Can &amp; PP in 440ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5060466519237,5060466515819,5060466513204,5060466513112,5060466513174,5060466513051,5060466513082</t>
   </si>
 </sst>
 </file>
@@ -543,7 +618,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -565,12 +640,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -622,7 +691,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -646,12 +715,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -700,7 +765,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -710,14 +775,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -740,19 +797,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -824,22 +876,23 @@
   </sheetPr>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.1488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.8279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,8 +1052,12 @@
       <c r="F7" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1127,7 +1184,9 @@
       <c r="F13" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="n">
+        <v>14</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1150,7 +1209,9 @@
       <c r="F14" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4" t="n">
+        <v>11</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1175,19 +1236,19 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1233,35 +1294,34 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="71.8697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="71.7441860465116"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.6418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="79.8651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="74.0837209302326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="73.8372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="82.3302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,7 +1903,15 @@
       <c r="M14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="8"/>
+      <c r="O14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1873,7 +1941,15 @@
       <c r="M15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q15" s="8"/>
+      <c r="O15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -1902,6 +1978,15 @@
       </c>
       <c r="M16" s="11" t="s">
         <v>67</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,6 +2451,120 @@
         <v>14</v>
       </c>
       <c r="Q27" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="8" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2386,23 +2585,23 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.693023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,6 +2683,9 @@
         <v>96</v>
       </c>
       <c r="D4" s="8"/>
+      <c r="E4" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="F4" s="11" t="s">
         <v>62</v>
       </c>
@@ -2682,14 +2884,14 @@
         <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>62</v>
@@ -2699,19 +2901,16 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>32</v>
+      <c r="A16" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="F16" s="11" t="s">
         <v>62</v>
       </c>
@@ -2720,160 +2919,175 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
+      <c r="A17" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D17" s="8"/>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="F17" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="8"/>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D19" s="8"/>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D20" s="8"/>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D21" s="8"/>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>38</v>
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D22" s="8"/>
+      <c r="F22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D38" s="8"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2892,31 +3106,31 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.186046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.6558139534884"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3674418604651"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.386046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.5209302325581"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.693023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,34 +3144,34 @@
         <v>47</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>42</v>
@@ -2978,27 +3192,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="171" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>65</v>
+      <c r="D2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>65</v>
@@ -3016,21 +3230,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>65</v>
+        <v>120</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>61</v>
@@ -3059,10 +3273,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>50</v>
@@ -3071,12 +3285,48 @@
         <v>62</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="S4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3097,35 +3347,35 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -3151,14 +3401,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>128</v>
+      <c r="B2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>4</v>
@@ -3183,14 +3433,14 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>129</v>
+      <c r="B3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -3215,14 +3465,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>130</v>
+      <c r="B4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3237,7 +3487,7 @@
         <v>67</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>22</v>
@@ -3247,14 +3497,14 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>128</v>
+      <c r="B5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -3279,14 +3529,14 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>129</v>
+      <c r="B6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -3311,14 +3561,14 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>130</v>
+      <c r="B7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3333,12 +3583,108 @@
         <v>92</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="0" t="s">
+      <c r="D9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3359,32 +3705,32 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P13" activeCellId="0" sqref="P13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P31" activeCellId="0" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.4372093023256"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="47.5023255813954"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.7720930232558"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.72093023255814"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.15348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.7674418604651"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="72.7302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1348837209302"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="74.9441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3741,7 @@
         <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>47</v>
@@ -3448,22 +3794,22 @@
         <v>12</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -3486,7 +3832,7 @@
         <v>14</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,10 +3840,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>59</v>
@@ -3519,28 +3865,28 @@
       <c r="Q3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" s="11" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R3" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D4" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>143</v>
+      <c r="F4" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="K4" s="11" t="n">
         <v>2</v>
@@ -3554,6 +3900,9 @@
       <c r="N4" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O4" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="P4" s="11" t="s">
         <v>22</v>
       </c>
@@ -3561,33 +3910,33 @@
         <v>14</v>
       </c>
       <c r="R4" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="5" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>146</v>
-      </c>
       <c r="K5" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L5" s="11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M5" s="11" t="s">
         <v>62</v>
@@ -3595,6 +3944,9 @@
       <c r="N5" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O5" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="P5" s="11" t="s">
         <v>22</v>
       </c>
@@ -3602,18 +3954,18 @@
         <v>14</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>147</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>59</v>
@@ -3621,14 +3973,14 @@
       <c r="E6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="19" t="s">
         <v>148</v>
       </c>
       <c r="K6" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>62</v>
@@ -3636,6 +3988,9 @@
       <c r="N6" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O6" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="P6" s="11" t="s">
         <v>22</v>
       </c>
@@ -3643,18 +3998,18 @@
         <v>14</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>149</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>59</v>
@@ -3662,14 +4017,14 @@
       <c r="E7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>83</v>
+      <c r="F7" s="19" t="s">
+        <v>150</v>
       </c>
       <c r="K7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>62</v>
@@ -3677,6 +4032,9 @@
       <c r="N7" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O7" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="P7" s="11" t="s">
         <v>22</v>
       </c>
@@ -3684,27 +4042,33 @@
         <v>14</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>85</v>
-      </c>
       <c r="K8" s="11" t="n">
         <v>2</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>8</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>62</v>
@@ -3712,6 +4076,9 @@
       <c r="N8" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O8" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="P8" s="11" t="s">
         <v>22</v>
       </c>
@@ -3719,33 +4086,33 @@
         <v>14</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>155</v>
-      </c>
       <c r="K9" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="11" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M9" s="11" t="s">
         <v>62</v>
@@ -3753,6 +4120,9 @@
       <c r="N9" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O9" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="P9" s="11" t="s">
         <v>22</v>
       </c>
@@ -3760,18 +4130,18 @@
         <v>14</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>157</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>59</v>
@@ -3779,14 +4149,18 @@
       <c r="E10" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="F10" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M10" s="11" t="s">
         <v>62</v>
@@ -3801,18 +4175,18 @@
         <v>14</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>160</v>
+      <c r="A11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>59</v>
@@ -3820,14 +4194,14 @@
       <c r="E11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="K11" s="0" t="n">
+      <c r="F11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L11" s="11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>62</v>
@@ -3836,24 +4210,21 @@
         <v>67</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>140</v>
+        <v>21</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>59</v>
@@ -3861,14 +4232,11 @@
       <c r="E12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L12" s="11" t="n">
-        <v>1</v>
+      <c r="F12" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="11" t="n">
+        <v>2</v>
       </c>
       <c r="M12" s="11" t="s">
         <v>62</v>
@@ -3877,39 +4245,39 @@
         <v>67</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="11" t="s">
         <v>14</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>140</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>2</v>
+        <v>159</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K13" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="L13" s="11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13" s="11" t="s">
         <v>62</v>
@@ -3918,39 +4286,39 @@
         <v>67</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>167</v>
+        <v>65</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="K14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="L14" s="11" t="n">
-        <v>2</v>
       </c>
       <c r="M14" s="11" t="s">
         <v>62</v>
@@ -3958,9 +4326,6 @@
       <c r="N14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="O14" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="P14" s="11" t="s">
         <v>22</v>
       </c>
@@ -3968,33 +4333,33 @@
         <v>14</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>167</v>
-      </c>
       <c r="K15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="L15" s="11" t="n">
-        <v>2</v>
       </c>
       <c r="M15" s="11" t="s">
         <v>62</v>
@@ -4002,41 +4367,40 @@
       <c r="N15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="P15" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="11" t="s">
         <v>14</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F16" s="22"/>
       <c r="K16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L16" s="11" t="n">
         <v>1</v>
-      </c>
-      <c r="L16" s="11" t="n">
-        <v>2</v>
       </c>
       <c r="M16" s="11" t="s">
         <v>62</v>
@@ -4044,90 +4408,90 @@
       <c r="N16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="O16" s="0" t="s">
-        <v>131</v>
-      </c>
       <c r="P16" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="Q16" s="11" t="s">
         <v>14</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" s="11" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D17" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="K17" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="L17" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="P17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>59</v>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>171</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="K18" s="11" t="n">
-        <v>2</v>
+        <v>159</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="L18" s="11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>22</v>
@@ -4136,39 +4500,42 @@
         <v>14</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>59</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>171</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="K19" s="11" t="n">
-        <v>2</v>
+        <v>159</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="L19" s="11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M19" s="11" t="s">
         <v>62</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>22</v>
@@ -4177,33 +4544,42 @@
         <v>14</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>59</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>173</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="K20" s="11" t="n">
+        <v>159</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="11" t="n">
         <v>2</v>
       </c>
       <c r="M20" s="11" t="s">
         <v>62</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>133</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>22</v>
@@ -4212,33 +4588,33 @@
         <v>14</v>
       </c>
       <c r="R20" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>152</v>
+      <c r="C21" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>155</v>
+        <v>65</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="K21" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21" s="11" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M21" s="11" t="s">
         <v>62</v>
@@ -4246,6 +4622,9 @@
       <c r="N21" s="11" t="s">
         <v>92</v>
       </c>
+      <c r="O21" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="P21" s="11" t="s">
         <v>22</v>
       </c>
@@ -4253,7 +4632,1333 @@
         <v>14</v>
       </c>
       <c r="R21" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" s="11" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K22" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L22" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K23" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L23" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" s="11" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K25" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L25" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L26" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L27" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R28" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>156</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K30" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R30" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L31" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L32" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R32" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L33" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P33" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R33" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L34" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P34" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q34" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R34" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M37" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M38" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O38" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q38" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R38" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L39" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N39" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R39" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L40" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M40" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R40" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L41" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N41" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="P41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R41" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L42" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N42" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q42" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R42" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q43" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L44" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M44" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q44" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R44" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L45" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M45" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N45" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O45" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q45" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R45" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L46" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M46" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N46" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O46" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q46" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R46" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L47" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M47" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O47" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R47" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L48" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O48" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="P48" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q48" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R48" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L49" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O49" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q49" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R49" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L50" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N50" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O50" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="P50" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q50" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R50" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M51" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P51" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R51" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K52" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L52" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P52" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q52" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R52" s="8" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes after debugging L&T
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">ALL SSD IC, SSD FC, Twist and Stills must be greater than 50% of All Competitor SSD IC &amp; SSD FC Flavours and Stills</t>
   </si>
   <si>
-    <t xml:space="preserve">CCBSA &amp; DOC Coolers</t>
+    <t xml:space="preserve">CCBSA,DOC Coolers</t>
   </si>
   <si>
     <t xml:space="preserve">Min 4 x Cooler Doors</t>
@@ -877,22 +877,22 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3953488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1236,16 +1236,16 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,27 +1301,28 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="74.0837209302326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="73.8372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="82.3302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="76.2976744186047"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="76.0511627906977"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="84.7906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,15 +2594,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.1441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.306976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,29 +3109,29 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.386046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.693023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.711627906977"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,17 +3356,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3707,30 +3708,29 @@
   </sheetPr>
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P31" activeCellId="0" sqref="P31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.7720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.8325581395349"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6139534883721"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1348837209302"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="74.9441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.506976744186"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="77.2837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4368,7 +4368,7 @@
         <v>67</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q15" s="11" t="s">
         <v>14</v>
@@ -4409,7 +4409,7 @@
         <v>67</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q16" s="11" t="s">
         <v>14</v>
@@ -4450,7 +4450,7 @@
         <v>67</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="11" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
adding by scene calculation logic
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,9 @@
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$R$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -103,7 +105,7 @@
     <t xml:space="preserve">SSD FC Diets</t>
   </si>
   <si>
-    <t xml:space="preserve">Stills - Energy </t>
+    <t xml:space="preserve">Stills – Energy</t>
   </si>
   <si>
     <t xml:space="preserve">Stills - Energy Poster</t>
@@ -304,7 +306,7 @@
     <t xml:space="preserve">6001134297308,5449000166241,6001134087305,5449000117977,6001134687307</t>
   </si>
   <si>
-    <t xml:space="preserve">Price compliance: 2L Twist </t>
+    <t xml:space="preserve">Price compliance: 2L Twist</t>
   </si>
   <si>
     <t xml:space="preserve">5449000098580,5449000060082</t>
@@ -526,6 +528,9 @@
     <t xml:space="preserve">90375149,5449000052131,5449000224453,5449000246295,5449000157751,5449000230188</t>
   </si>
   <si>
+    <t xml:space="preserve">SSD IC Diets Availability of: 200ml CAN, 300 ml PET CZ,STZ)</t>
+  </si>
+  <si>
     <t xml:space="preserve">90375149,5449000052131,5449000224453,5449000246295</t>
   </si>
   <si>
@@ -647,9 +652,6 @@
   </si>
   <si>
     <t xml:space="preserve">SSD Diets Brands/Packs: 1.5L in (CZ/SZ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills - Energy</t>
   </si>
   <si>
     <t xml:space="preserve">Stills Availability of Burn in 500ml Can &amp; PP in 440ml</t>
@@ -978,27 +980,27 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.1627906976744"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.2558139534884"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1282,7 +1284,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1306,7 +1308,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1336,7 +1338,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1383,16 +1385,16 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,36 +1445,36 @@
   </sheetPr>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B52" activeCellId="0" sqref="B52"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="76.2976744186047"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="76.0511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="84.7906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="80.8511627906977"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="80.6046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="89.8372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1558,7 +1560,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1732,7 +1734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1777,7 +1779,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -1948,7 +1950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
@@ -2023,7 +2025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>29</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>31</v>
       </c>
@@ -2099,7 +2101,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>31</v>
       </c>
@@ -2137,7 +2139,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
@@ -2179,7 +2181,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
@@ -2266,7 +2268,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
@@ -2311,7 +2313,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
@@ -2567,7 +2569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>23</v>
       </c>
@@ -2602,7 +2604,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>29</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>31</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
         <v>18</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -2800,7 +2802,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
         <v>18</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
         <v>18</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
         <v>20</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
         <v>21</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
         <v>21</v>
       </c>
@@ -3012,7 +3014,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
         <v>21</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
         <v>22</v>
       </c>
@@ -3088,7 +3090,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
         <v>21</v>
       </c>
@@ -3126,7 +3128,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
         <v>22</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
         <v>21</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
         <v>22</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>23</v>
       </c>
@@ -3288,7 +3290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>23</v>
       </c>
@@ -3327,7 +3329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>29</v>
       </c>
@@ -3403,7 +3405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>31</v>
       </c>
@@ -3441,7 +3443,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
         <v>18</v>
       </c>
@@ -3483,7 +3485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
         <v>18</v>
       </c>
@@ -3525,7 +3527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
         <v>18</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
         <v>18</v>
       </c>
@@ -3615,7 +3617,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
         <v>20</v>
       </c>
@@ -3658,7 +3660,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
         <v>21</v>
       </c>
@@ -3696,7 +3698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
         <v>21</v>
       </c>
@@ -3737,7 +3739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
         <v>21</v>
       </c>
@@ -3775,7 +3777,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
         <v>22</v>
       </c>
@@ -3813,7 +3815,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
         <v>21</v>
       </c>
@@ -3851,7 +3853,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
         <v>22</v>
       </c>
@@ -3892,7 +3894,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
         <v>21</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
         <v>22</v>
       </c>
@@ -3974,7 +3976,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>23</v>
       </c>
@@ -4013,7 +4015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>23</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>29</v>
       </c>
@@ -4094,7 +4096,7 @@
       <c r="A65" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="11" t="s">
         <v>90</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -4128,7 +4130,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>31</v>
       </c>
@@ -4170,7 +4172,7 @@
   <autoFilter ref="A1:Q66"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4187,24 +4189,24 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -4230,7 +4232,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
@@ -4253,7 +4255,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -4276,7 +4278,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -4299,7 +4301,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -4322,7 +4324,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
@@ -4362,7 +4364,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>33</v>
       </c>
@@ -4383,7 +4385,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>33</v>
       </c>
@@ -4406,7 +4408,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>33</v>
       </c>
@@ -4427,7 +4429,7 @@
       </c>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -4447,7 +4449,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>33</v>
       </c>
@@ -4470,7 +4472,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>33</v>
       </c>
@@ -4493,7 +4495,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>33</v>
       </c>
@@ -4516,7 +4518,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -4536,7 +4538,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>33</v>
       </c>
@@ -4555,7 +4557,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>33</v>
       </c>
@@ -4591,34 +4593,34 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.4697674418605"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.711627906977"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="120.725581395349"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.6093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -4677,7 +4679,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
@@ -4715,7 +4717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -4753,11 +4755,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="11" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -4787,7 +4789,6 @@
       <c r="S4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ4" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4808,26 +4809,26 @@
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -4859,7 +4860,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -4891,7 +4892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
@@ -4923,7 +4924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
@@ -4955,7 +4956,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
         <v>13</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
@@ -5147,7 +5148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>13</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
         <v>13</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
@@ -5260,25 +5261,37 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:76"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.3581395348837"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="18" min="7" style="0" width="10.5023255813953"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="177.33023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.61395348837209"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.87441860465116"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.61395348837209"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.24651162790698"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="75.1906976744186"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -5334,7 +5347,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -5380,7 +5393,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -5414,7 +5427,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -5457,10 +5470,8 @@
       <c r="R4" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="11" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -5503,10 +5514,8 @@
       <c r="R5" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -5550,7 +5559,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -5594,7 +5603,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -5638,12 +5647,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>155</v>
@@ -5655,7 +5664,7 @@
         <v>66</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K9" s="11" t="n">
         <v>2</v>
@@ -5682,12 +5691,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>155</v>
@@ -5699,7 +5708,7 @@
         <v>66</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -5727,12 +5736,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>155</v>
@@ -5768,12 +5777,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -5804,24 +5813,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="E13" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K13" s="11" t="n">
         <v>1</v>
@@ -5842,15 +5851,15 @@
         <v>15</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>155</v>
@@ -5862,7 +5871,7 @@
         <v>66</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>2</v>
@@ -5883,15 +5892,15 @@
         <v>15</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>155</v>
@@ -5903,7 +5912,7 @@
         <v>66</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>2</v>
@@ -5927,12 +5936,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>155</v>
@@ -5944,7 +5953,7 @@
         <v>66</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>2</v>
@@ -5968,12 +5977,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>155</v>
@@ -5985,7 +5994,7 @@
         <v>66</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>2</v>
@@ -6009,24 +6018,24 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>1</v>
@@ -6050,27 +6059,27 @@
         <v>15</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>1</v>
@@ -6094,27 +6103,27 @@
         <v>15</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>1</v>
@@ -6138,10 +6147,10 @@
         <v>15</v>
       </c>
       <c r="R20" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" s="11" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
@@ -6184,10 +6193,8 @@
       <c r="R21" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
-    </row>
-    <row r="22" s="11" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" s="11" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>18</v>
       </c>
@@ -6230,10 +6237,8 @@
       <c r="R22" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>18</v>
       </c>
@@ -6277,7 +6282,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -6321,7 +6326,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>20</v>
       </c>
@@ -6365,12 +6370,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>155</v>
@@ -6382,7 +6387,7 @@
         <v>66</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K26" s="11" t="n">
         <v>2</v>
@@ -6409,12 +6414,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>155</v>
@@ -6426,7 +6431,7 @@
         <v>66</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -6454,12 +6459,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>155</v>
@@ -6495,12 +6500,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -6531,24 +6536,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C30" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="E30" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K30" s="11" t="n">
         <v>1</v>
@@ -6569,15 +6574,15 @@
         <v>15</v>
       </c>
       <c r="R30" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>155</v>
@@ -6589,7 +6594,7 @@
         <v>66</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K31" s="0" t="n">
         <v>2</v>
@@ -6610,15 +6615,15 @@
         <v>15</v>
       </c>
       <c r="R31" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>155</v>
@@ -6630,7 +6635,7 @@
         <v>66</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>2</v>
@@ -6654,12 +6659,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>155</v>
@@ -6671,7 +6676,7 @@
         <v>66</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K33" s="0" t="n">
         <v>2</v>
@@ -6695,12 +6700,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>155</v>
@@ -6712,7 +6717,7 @@
         <v>66</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K34" s="0" t="n">
         <v>2</v>
@@ -6736,24 +6741,24 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>1</v>
@@ -6774,27 +6779,27 @@
         <v>15</v>
       </c>
       <c r="R35" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K36" s="0" t="n">
         <v>1</v>
@@ -6818,27 +6823,27 @@
         <v>15</v>
       </c>
       <c r="R36" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>1</v>
@@ -6862,27 +6867,27 @@
         <v>15</v>
       </c>
       <c r="R37" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K38" s="0" t="n">
         <v>1</v>
@@ -6906,15 +6911,15 @@
         <v>15</v>
       </c>
       <c r="R38" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>155</v>
@@ -6926,7 +6931,7 @@
         <v>66</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K39" s="0" t="n">
         <v>2</v>
@@ -6953,12 +6958,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>155</v>
@@ -6970,7 +6975,7 @@
         <v>66</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K40" s="0" t="n">
         <v>2</v>
@@ -6997,12 +7002,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>155</v>
@@ -7014,7 +7019,7 @@
         <v>66</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K41" s="0" t="n">
         <v>2</v>
@@ -7041,12 +7046,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>155</v>
@@ -7058,7 +7063,7 @@
         <v>66</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K42" s="0" t="n">
         <v>2</v>
@@ -7085,12 +7090,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>155</v>
@@ -7102,7 +7107,7 @@
         <v>66</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K43" s="0" t="n">
         <v>2</v>
@@ -7129,12 +7134,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>155</v>
@@ -7146,7 +7151,7 @@
         <v>66</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K44" s="0" t="n">
         <v>2</v>
@@ -7173,12 +7178,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>155</v>
@@ -7190,7 +7195,7 @@
         <v>66</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K45" s="0" t="n">
         <v>2</v>
@@ -7217,12 +7222,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>155</v>
@@ -7234,7 +7239,7 @@
         <v>66</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K46" s="0" t="n">
         <v>2</v>
@@ -7261,12 +7266,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>155</v>
@@ -7278,7 +7283,7 @@
         <v>66</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K47" s="0" t="n">
         <v>2</v>
@@ -7305,12 +7310,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>155</v>
@@ -7322,7 +7327,7 @@
         <v>66</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K48" s="0" t="n">
         <v>2</v>
@@ -7349,12 +7354,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>155</v>
@@ -7366,7 +7371,7 @@
         <v>66</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K49" s="0" t="n">
         <v>2</v>
@@ -7393,12 +7398,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>155</v>
@@ -7439,7 +7444,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>206</v>
@@ -7475,24 +7480,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C52" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="E52" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K52" s="11" t="n">
         <v>1</v>
@@ -7513,10 +7518,10 @@
         <v>15</v>
       </c>
       <c r="R52" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>27</v>
       </c>
@@ -7533,7 +7538,7 @@
         <v>66</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K53" s="0" t="n">
         <v>2</v>
@@ -7554,10 +7559,10 @@
         <v>15</v>
       </c>
       <c r="R53" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>27</v>
       </c>
@@ -7574,7 +7579,7 @@
         <v>66</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K54" s="0" t="n">
         <v>2</v>
@@ -7595,10 +7600,10 @@
         <v>15</v>
       </c>
       <c r="R54" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>27</v>
       </c>
@@ -7615,7 +7620,7 @@
         <v>66</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K55" s="0" t="n">
         <v>2</v>
@@ -7636,10 +7641,10 @@
         <v>15</v>
       </c>
       <c r="R55" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>27</v>
       </c>
@@ -7677,10 +7682,10 @@
         <v>15</v>
       </c>
       <c r="R56" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>27</v>
       </c>
@@ -7718,15 +7723,15 @@
         <v>15</v>
       </c>
       <c r="R57" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>155</v>
@@ -7738,7 +7743,7 @@
         <v>66</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K58" s="0" t="n">
         <v>2</v>
@@ -7765,12 +7770,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>155</v>
@@ -7782,7 +7787,7 @@
         <v>66</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K59" s="0" t="n">
         <v>2</v>
@@ -7809,12 +7814,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>155</v>
@@ -7826,7 +7831,7 @@
         <v>66</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K60" s="0" t="n">
         <v>2</v>
@@ -7853,12 +7858,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>155</v>
@@ -7870,7 +7875,7 @@
         <v>66</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K61" s="0" t="n">
         <v>2</v>
@@ -7897,12 +7902,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>155</v>
@@ -7914,7 +7919,7 @@
         <v>66</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K62" s="0" t="n">
         <v>2</v>
@@ -7941,12 +7946,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>155</v>
@@ -7958,7 +7963,7 @@
         <v>66</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K63" s="0" t="n">
         <v>2</v>
@@ -7985,12 +7990,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>155</v>
@@ -8002,7 +8007,7 @@
         <v>66</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K64" s="0" t="n">
         <v>2</v>
@@ -8029,12 +8034,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>155</v>
@@ -8046,7 +8051,7 @@
         <v>66</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K65" s="0" t="n">
         <v>2</v>
@@ -8073,12 +8078,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>155</v>
@@ -8090,7 +8095,7 @@
         <v>66</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K66" s="0" t="n">
         <v>2</v>
@@ -8117,12 +8122,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>155</v>
@@ -8134,7 +8139,7 @@
         <v>66</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K67" s="0" t="n">
         <v>2</v>
@@ -8161,12 +8166,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>155</v>
@@ -8178,7 +8183,7 @@
         <v>66</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K68" s="0" t="n">
         <v>2</v>
@@ -8205,12 +8210,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>155</v>
@@ -8251,7 +8256,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>206</v>
@@ -8287,24 +8292,24 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C71" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D71" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="E71" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F71" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K71" s="11" t="n">
         <v>1</v>
@@ -8325,10 +8330,10 @@
         <v>15</v>
       </c>
       <c r="R71" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>27</v>
       </c>
@@ -8345,7 +8350,7 @@
         <v>66</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K72" s="0" t="n">
         <v>2</v>
@@ -8366,10 +8371,10 @@
         <v>15</v>
       </c>
       <c r="R72" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>27</v>
       </c>
@@ -8386,7 +8391,7 @@
         <v>66</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K73" s="0" t="n">
         <v>2</v>
@@ -8407,10 +8412,10 @@
         <v>15</v>
       </c>
       <c r="R73" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>27</v>
       </c>
@@ -8427,7 +8432,7 @@
         <v>66</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K74" s="0" t="n">
         <v>2</v>
@@ -8448,10 +8453,10 @@
         <v>15</v>
       </c>
       <c r="R74" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>27</v>
       </c>
@@ -8489,10 +8494,10 @@
         <v>15</v>
       </c>
       <c r="R75" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>27</v>
       </c>
@@ -8530,7 +8535,7 @@
         <v>15</v>
       </c>
       <c r="R76" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding temporary solution to enter scene-session hierarchy availability, common.kpi_repults - make sure that it does not run into index error if no queries
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,8 +21,10 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -986,18 +988,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.1953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.2558139534884"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.3627906976744"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,10 +1393,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,23 +1457,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="80.8511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="80.6046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="89.8372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="83.3116279069767"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="83.0651162790698"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="92.5441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4195,15 +4197,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4601,23 +4603,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="120.725581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="124.413953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4809,23 +4811,23 @@
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5263,32 +5265,32 @@
   </sheetPr>
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G19" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P35" activeCellId="0" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="177.33023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.61395348837209"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.61395348837209"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="75.1906976744186"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.8744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="182.748837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="77.5302325581395"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6650,7 +6652,7 @@
         <v>94</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q32" s="11" t="s">
         <v>15</v>
@@ -6691,7 +6693,7 @@
         <v>94</v>
       </c>
       <c r="P33" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q33" s="11" t="s">
         <v>15</v>
@@ -6732,7 +6734,7 @@
         <v>94</v>
       </c>
       <c r="P34" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q34" s="11" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
amend LT template and change SOS logic to record the results in accordance with mock up
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,9 +22,13 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -107,7 +111,7 @@
     <t xml:space="preserve">SSD FC Diets</t>
   </si>
   <si>
-    <t xml:space="preserve">Stills – Energy</t>
+    <t xml:space="preserve">Stills-Energy</t>
   </si>
   <si>
     <t xml:space="preserve">Stills - Energy Poster</t>
@@ -461,10 +465,10 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
-    <t xml:space="preserve">SSD IC, SSD FC, Twist and Stills greater than 50% of Competitor SSD IC &amp; SSD FC Flavours and Stills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCBSA, DOC Coolers</t>
+    <t xml:space="preserve">SSD IC, SSD FC, Twist and Stills greater than 50% of Competitor of category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCBSA Cooler, DOC Coolers</t>
   </si>
   <si>
     <t xml:space="preserve">Min 4 x Cooler Doors</t>
@@ -983,23 +987,23 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.8279069767442"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,10 +1397,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,32 +1452,32 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="83.3116279069767"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="83.0651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="92.5441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="88.3581395348837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="88.2372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="98.0790697674419"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,8 +1996,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -2571,8 +2575,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -3253,8 +3257,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -3292,8 +3296,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -3978,8 +3982,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B62" s="11" t="s">
@@ -4017,8 +4021,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B63" s="11" t="s">
@@ -4197,15 +4201,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.8976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.2046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,31 +4599,31 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="124.413953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="132.046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.0558139534884"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4792,6 +4796,8 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4817,17 +4823,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.6418604651163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5265,32 +5271,32 @@
   </sheetPr>
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G19" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P35" activeCellId="0" sqref="P35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="87.9906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="182.748837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="77.5302325581395"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.5255813953488"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="193.944186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.98139534883721"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="82.3302325581395"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5780,7 +5786,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -6502,8 +6508,8 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
@@ -7445,7 +7451,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B51" s="0" t="s">
@@ -8257,7 +8263,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="0" t="s">

</xml_diff>

<commit_message>
new update LT template, start tests to fit the code
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_L&T.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,11 +19,11 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">Price!$A$1:$Q$66</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Price!$A$1:$Q$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="dcsvx" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$R$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$R$116</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$R$116</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$R$76</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2742" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="244">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t xml:space="preserve">PP/Monster Energy pricing Poster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Pack Monster and Powerplay</t>
   </si>
   <si>
     <t xml:space="preserve">Stills Availability of (JJ) Cold</t>
@@ -891,7 +894,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1000,10 +1003,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1083,11 +1082,11 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7813953488372"/>
@@ -1103,7 +1102,7 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3209302325581"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1392,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1417,7 +1416,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1502,8 +1501,8 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1560,17 +1559,17 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:92"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F56" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="bottomRight" activeCell="B78" activeCellId="0" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4837209302326"/>
@@ -1591,7 +1590,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="103.986046511628"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1644,7 +1643,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -1896,7 +1895,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>29</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>31</v>
       </c>
@@ -2218,7 +2217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>31</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>18</v>
       </c>
@@ -2385,7 +2384,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>21</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
@@ -2721,7 +2720,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
         <v>29</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>31</v>
       </c>
@@ -2797,7 +2796,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>31</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
         <v>18</v>
       </c>
@@ -2877,7 +2876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
         <v>18</v>
       </c>
@@ -2919,7 +2918,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
         <v>18</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
         <v>18</v>
       </c>
@@ -3009,7 +3008,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
         <v>20</v>
       </c>
@@ -3052,7 +3051,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
         <v>21</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
         <v>21</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
         <v>21</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
         <v>22</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
         <v>21</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
         <v>22</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
         <v>21</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
         <v>22</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
@@ -3440,7 +3439,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="15" t="s">
         <v>29</v>
       </c>
@@ -3478,7 +3477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>31</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>31</v>
       </c>
@@ -3554,7 +3553,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
         <v>18</v>
       </c>
@@ -3596,7 +3595,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
         <v>18</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
         <v>18</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
         <v>18</v>
       </c>
@@ -3728,7 +3727,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
         <v>20</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
         <v>21</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
         <v>21</v>
       </c>
@@ -3850,7 +3849,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
         <v>21</v>
       </c>
@@ -3888,7 +3887,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
         <v>22</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
         <v>21</v>
       </c>
@@ -3964,7 +3963,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
         <v>22</v>
       </c>
@@ -4005,7 +4004,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
         <v>21</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
         <v>22</v>
       </c>
@@ -4087,7 +4086,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
         <v>23</v>
       </c>
@@ -4123,7 +4122,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
         <v>23</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
         <v>29</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>31</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>31</v>
       </c>
@@ -4273,7 +4272,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="15" t="s">
         <v>18</v>
       </c>
@@ -4310,9 +4309,8 @@
       <c r="Q67" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ67" s="0"/>
-    </row>
-    <row r="68" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="68" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
         <v>18</v>
       </c>
@@ -4349,9 +4347,8 @@
       <c r="Q68" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ68" s="0"/>
-    </row>
-    <row r="69" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="69" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
         <v>20</v>
       </c>
@@ -4388,9 +4385,8 @@
       <c r="Q69" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ69" s="0"/>
-    </row>
-    <row r="70" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
         <v>21</v>
       </c>
@@ -4427,9 +4423,8 @@
       <c r="Q70" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ70" s="0"/>
-    </row>
-    <row r="71" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="71" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
         <v>21</v>
       </c>
@@ -4466,9 +4461,8 @@
       <c r="Q71" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ71" s="0"/>
-    </row>
-    <row r="72" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="72" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
         <v>21</v>
       </c>
@@ -4505,9 +4499,8 @@
       <c r="Q72" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ72" s="0"/>
-    </row>
-    <row r="73" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="73" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
         <v>22</v>
       </c>
@@ -4544,9 +4537,8 @@
       <c r="Q73" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ73" s="0"/>
-    </row>
-    <row r="74" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="74" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
         <v>22</v>
       </c>
@@ -4583,9 +4575,8 @@
       <c r="Q74" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMJ74" s="0"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
         <v>23</v>
       </c>
@@ -4621,7 +4612,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
         <v>23</v>
       </c>
@@ -4657,7 +4648,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="15" t="s">
         <v>29</v>
       </c>
@@ -4695,7 +4686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="15" t="s">
         <v>31</v>
       </c>
@@ -4733,7 +4724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="15" t="s">
         <v>31</v>
       </c>
@@ -4771,7 +4762,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="15" t="s">
         <v>18</v>
       </c>
@@ -4809,7 +4800,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="15" t="s">
         <v>18</v>
       </c>
@@ -4847,7 +4838,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="15" t="s">
         <v>20</v>
       </c>
@@ -4885,7 +4876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
         <v>21</v>
       </c>
@@ -4923,7 +4914,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="15" t="s">
         <v>21</v>
       </c>
@@ -4961,7 +4952,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="15" t="s">
         <v>21</v>
       </c>
@@ -4999,7 +4990,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="15" t="s">
         <v>22</v>
       </c>
@@ -5037,7 +5028,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15" t="s">
         <v>22</v>
       </c>
@@ -5075,7 +5066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
@@ -5111,7 +5102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
@@ -5147,7 +5138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="15" t="s">
         <v>29</v>
       </c>
@@ -5185,7 +5176,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="15" t="s">
         <v>31</v>
       </c>
@@ -5223,7 +5214,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15" t="s">
         <v>31</v>
       </c>
@@ -5280,7 +5271,7 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6054,13 +6045,13 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7488372093023"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.4837209302326"/>
@@ -6080,7 +6071,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.906976744186"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -6139,7 +6130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
@@ -6177,7 +6168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -6215,7 +6206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
@@ -6249,7 +6240,6 @@
       <c r="S4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ4" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6270,11 +6260,11 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9674418604651"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5813953488372"/>
@@ -6286,7 +6276,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4139534883721"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -6318,7 +6308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -6351,7 +6341,7 @@
       </c>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
@@ -6383,7 +6373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
@@ -6415,7 +6405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
         <v>13</v>
       </c>
@@ -6447,7 +6437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
         <v>13</v>
       </c>
@@ -6479,7 +6469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
         <v>13</v>
       </c>
@@ -6511,7 +6501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -6543,7 +6533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
         <v>13</v>
       </c>
@@ -6575,7 +6565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
         <v>13</v>
       </c>
@@ -6607,7 +6597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
@@ -6639,7 +6629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
@@ -6671,7 +6661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
@@ -6703,7 +6693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
@@ -6735,7 +6725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
         <v>13</v>
       </c>
@@ -6767,7 +6757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
         <v>13</v>
       </c>
@@ -6799,7 +6789,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
         <v>13</v>
       </c>
@@ -6831,7 +6821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
         <v>13</v>
       </c>
@@ -6863,7 +6853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
@@ -6912,13 +6902,13 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:116"/>
+  <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L91" activeCellId="0" sqref="L91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2744186046512"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.1441860465116"/>
@@ -6940,7 +6930,7 @@
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="27.5674418604651"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -6996,7 +6986,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -7042,7 +7032,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -7076,7 +7066,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -7119,9 +7109,8 @@
       <c r="R4" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -7164,9 +7153,8 @@
       <c r="R5" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -7210,7 +7198,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
@@ -7254,7 +7242,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -7298,7 +7286,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
@@ -7342,7 +7330,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
@@ -7387,7 +7375,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
@@ -7428,7 +7416,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -7466,7 +7454,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
@@ -7507,7 +7495,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>27</v>
       </c>
@@ -7548,7 +7536,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
@@ -7589,7 +7577,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>27</v>
       </c>
@@ -7630,7 +7618,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>27</v>
       </c>
@@ -7671,7 +7659,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>33</v>
       </c>
@@ -7715,7 +7703,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
@@ -7759,7 +7747,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>33</v>
       </c>
@@ -7803,7 +7791,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
@@ -7846,9 +7834,8 @@
       <c r="R21" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AMJ21" s="0"/>
-    </row>
-    <row r="22" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>18</v>
       </c>
@@ -7891,9 +7878,8 @@
       <c r="R22" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AMJ22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>18</v>
       </c>
@@ -7937,7 +7923,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -7981,7 +7967,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
         <v>20</v>
       </c>
@@ -8025,7 +8011,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
         <v>20</v>
       </c>
@@ -8069,7 +8055,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
@@ -8114,7 +8100,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
         <v>22</v>
       </c>
@@ -8155,7 +8141,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
@@ -8193,7 +8179,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>24</v>
       </c>
@@ -8234,7 +8220,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>27</v>
       </c>
@@ -8275,7 +8261,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>27</v>
       </c>
@@ -8316,7 +8302,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>27</v>
       </c>
@@ -8357,7 +8343,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>27</v>
       </c>
@@ -8398,7 +8384,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>33</v>
       </c>
@@ -8439,7 +8425,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>33</v>
       </c>
@@ -8483,7 +8469,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>33</v>
       </c>
@@ -8527,7 +8513,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>33</v>
       </c>
@@ -8571,7 +8557,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>200</v>
       </c>
@@ -8615,7 +8601,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>200</v>
       </c>
@@ -8659,7 +8645,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>200</v>
       </c>
@@ -8703,7 +8689,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>20</v>
       </c>
@@ -8747,7 +8733,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>20</v>
       </c>
@@ -8791,7 +8777,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>20</v>
       </c>
@@ -8835,7 +8821,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>21</v>
       </c>
@@ -8879,7 +8865,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>21</v>
       </c>
@@ -8923,7 +8909,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>21</v>
       </c>
@@ -8967,7 +8953,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>22</v>
       </c>
@@ -9011,7 +8997,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>22</v>
       </c>
@@ -9055,7 +9041,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>22</v>
       </c>
@@ -9099,7 +9085,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -9137,7 +9123,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>24</v>
       </c>
@@ -9178,7 +9164,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>27</v>
       </c>
@@ -9219,7 +9205,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>27</v>
       </c>
@@ -9260,7 +9246,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>27</v>
       </c>
@@ -9301,7 +9287,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>27</v>
       </c>
@@ -9342,7 +9328,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>27</v>
       </c>
@@ -9383,7 +9369,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>200</v>
       </c>
@@ -9427,7 +9413,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>200</v>
       </c>
@@ -9471,7 +9457,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>200</v>
       </c>
@@ -9515,7 +9501,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>20</v>
       </c>
@@ -9559,7 +9545,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>20</v>
       </c>
@@ -9603,7 +9589,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>20</v>
       </c>
@@ -9647,7 +9633,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>21</v>
       </c>
@@ -9691,7 +9677,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>21</v>
       </c>
@@ -9735,7 +9721,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>21</v>
       </c>
@@ -9779,7 +9765,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>22</v>
       </c>
@@ -9823,7 +9809,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>22</v>
       </c>
@@ -9867,7 +9853,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>22</v>
       </c>
@@ -9911,7 +9897,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
         <v>23</v>
       </c>
@@ -9949,7 +9935,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>24</v>
       </c>
@@ -9990,7 +9976,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>27</v>
       </c>
@@ -10031,7 +10017,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>27</v>
       </c>
@@ -10072,7 +10058,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>27</v>
       </c>
@@ -10113,7 +10099,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>27</v>
       </c>
@@ -10154,7 +10140,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>27</v>
       </c>
@@ -10195,7 +10181,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" s="15" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="15" t="s">
         <v>33</v>
       </c>
@@ -10238,9 +10224,8 @@
       <c r="R77" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="AMJ77" s="0"/>
-    </row>
-    <row r="78" s="15" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="78" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="15" t="s">
         <v>33</v>
       </c>
@@ -10283,9 +10268,8 @@
       <c r="R78" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="AMJ78" s="0"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="15" t="s">
         <v>33</v>
       </c>
@@ -10329,7 +10313,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="15" t="s">
         <v>33</v>
       </c>
@@ -10373,7 +10357,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="15" t="s">
         <v>33</v>
       </c>
@@ -10417,7 +10401,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="15" t="s">
         <v>33</v>
       </c>
@@ -10461,7 +10445,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
         <v>18</v>
       </c>
@@ -10502,7 +10486,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="15" t="s">
         <v>20</v>
       </c>
@@ -10546,7 +10530,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="15" t="s">
         <v>20</v>
       </c>
@@ -10590,7 +10574,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="15" t="s">
         <v>20</v>
       </c>
@@ -10634,7 +10618,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15" t="s">
         <v>21</v>
       </c>
@@ -10678,7 +10662,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="15" t="s">
         <v>21</v>
       </c>
@@ -10722,7 +10706,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="15" t="s">
         <v>21</v>
       </c>
@@ -10766,7 +10750,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="15" t="s">
         <v>22</v>
       </c>
@@ -10807,7 +10791,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
         <v>23</v>
       </c>
@@ -10845,7 +10829,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15" t="s">
         <v>24</v>
       </c>
@@ -10861,7 +10845,9 @@
       <c r="E92" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="F92" s="27"/>
+      <c r="F92" s="14" t="s">
+        <v>238</v>
+      </c>
       <c r="K92" s="15" t="n">
         <v>1</v>
       </c>
@@ -10884,12 +10870,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>165</v>
@@ -10925,12 +10911,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>165</v>
@@ -10942,7 +10928,7 @@
         <v>66</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K94" s="15" t="n">
         <v>2</v>
@@ -10966,12 +10952,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>165</v>
@@ -11007,12 +10993,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>165</v>
@@ -11048,7 +11034,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="15" t="s">
         <v>33</v>
       </c>
@@ -11092,7 +11078,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="15" t="s">
         <v>33</v>
       </c>
@@ -11140,7 +11126,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="15" t="s">
         <v>33</v>
       </c>
@@ -11188,7 +11174,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" s="15" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="15" t="s">
         <v>18</v>
       </c>
@@ -11228,9 +11214,8 @@
       <c r="R100" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="AMJ100" s="0"/>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="15" t="s">
         <v>20</v>
       </c>
@@ -11278,7 +11263,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="15" t="s">
         <v>20</v>
       </c>
@@ -11322,7 +11307,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="15" t="s">
         <v>20</v>
       </c>
@@ -11366,7 +11351,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="15" t="s">
         <v>21</v>
       </c>
@@ -11410,7 +11395,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="15" t="s">
         <v>21</v>
       </c>
@@ -11454,7 +11439,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="15" t="s">
         <v>21</v>
       </c>
@@ -11498,7 +11483,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="15" t="s">
         <v>22</v>
       </c>
@@ -11539,7 +11524,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
         <v>23</v>
       </c>
@@ -11577,7 +11562,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="15" t="s">
         <v>24</v>
       </c>
@@ -11593,7 +11578,9 @@
       <c r="E109" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="F109" s="27"/>
+      <c r="F109" s="14" t="s">
+        <v>238</v>
+      </c>
       <c r="K109" s="15" t="n">
         <v>1</v>
       </c>
@@ -11616,12 +11603,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>165</v>
@@ -11657,12 +11644,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C111" s="15" t="s">
         <v>165</v>
@@ -11674,7 +11661,7 @@
         <v>66</v>
       </c>
       <c r="F111" s="18" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K111" s="15" t="n">
         <v>2</v>
@@ -11698,12 +11685,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C112" s="15" t="s">
         <v>165</v>
@@ -11739,12 +11726,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C113" s="15" t="s">
         <v>165</v>
@@ -11780,7 +11767,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="15" t="s">
         <v>33</v>
       </c>
@@ -11824,7 +11811,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="15" t="s">
         <v>33</v>
       </c>
@@ -11872,7 +11859,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="15" t="s">
         <v>33</v>
       </c>

</xml_diff>